<commit_message>
latesd updates (official,sendMails,edit emp)
</commit_message>
<xml_diff>
--- a/HRBackend/uploads/penta3d.xlsx
+++ b/HRBackend/uploads/penta3d.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ATT\2023\Oct 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ATT\2023\Oct 2023\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACCBC737-42A5-4A41-87B7-87144C366229}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75B3B401-7A8E-4A16-978B-C49595025110}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AttendanceRecord" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="190">
   <si>
     <t>Employee ID</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Department</t>
+  </si>
+  <si>
     <t>2023/09/21</t>
   </si>
   <si>
@@ -115,7 +118,7 @@
     <t>2023/10/19</t>
   </si>
   <si>
-    <t>2023/10/20</t>
+    <t>Company</t>
   </si>
   <si>
     <t>--:-- --:--
@@ -1481,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1497,7 +1500,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1593,61 +1596,61 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>38</v>
@@ -1662,13 +1665,13 @@
         <v>41</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>43</v>
@@ -1683,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="63" customHeight="1">
@@ -1691,19 +1694,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>50</v>
@@ -1715,37 +1718,37 @@
         <v>52</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>54</v>
@@ -1760,13 +1763,13 @@
         <v>57</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="AB3" s="4" t="s">
         <v>59</v>
@@ -1781,7 +1784,7 @@
         <v>62</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="63" customHeight="1">
@@ -1789,40 +1792,40 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>65</v>
@@ -1834,52 +1837,52 @@
         <v>67</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="AE4" s="1" t="s">
         <v>69</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="63" customHeight="1">
@@ -1887,19 +1890,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>73</v>
@@ -1911,37 +1914,37 @@
         <v>75</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="U5" s="4" t="s">
         <v>77</v>
@@ -1956,13 +1959,13 @@
         <v>80</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>82</v>
@@ -1974,10 +1977,10 @@
         <v>84</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="63" customHeight="1">
@@ -1985,97 +1988,97 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>87</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="AB6" s="1" t="s">
         <v>90</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="63" customHeight="1">
@@ -2083,40 +2086,40 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>93</v>
@@ -2128,52 +2131,52 @@
         <v>95</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="AB7" s="4" t="s">
         <v>98</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="AD7" s="4" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="AE7" s="4" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="63" customHeight="1">
@@ -2181,61 +2184,61 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>103</v>
@@ -2250,28 +2253,28 @@
         <v>106</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="AB8" s="1" t="s">
         <v>108</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="AE8" s="1" t="s">
         <v>110</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="63" customHeight="1">
@@ -2279,97 +2282,97 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AF9" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="63" customHeight="1">
@@ -2377,61 +2380,61 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>115</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>118</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>120</v>
@@ -2446,28 +2449,28 @@
         <v>123</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>126</v>
+        <v>33</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="63" customHeight="1">
@@ -2475,97 +2478,97 @@
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AB11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AF11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="63" customHeight="1">
@@ -2573,97 +2576,97 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>131</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>133</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>123</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="63" customHeight="1">
@@ -2671,61 +2674,61 @@
         <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>138</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>141</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>143</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>145</v>
+        <v>33</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>146</v>
@@ -2740,28 +2743,28 @@
         <v>149</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="AB13" s="4" t="s">
         <v>151</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="AD13" s="4" t="s">
-        <v>152</v>
+        <v>33</v>
       </c>
       <c r="AE13" s="4" t="s">
         <v>153</v>
       </c>
       <c r="AF13" s="4" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="63" customHeight="1">
@@ -2769,19 +2772,19 @@
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>157</v>
@@ -2793,16 +2796,16 @@
         <v>159</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>161</v>
@@ -2814,37 +2817,37 @@
         <v>163</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>164</v>
+        <v>33</v>
       </c>
       <c r="AB14" s="4" t="s">
         <v>165</v>
@@ -2859,7 +2862,7 @@
         <v>168</v>
       </c>
       <c r="AF14" s="4" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="63" customHeight="1">
@@ -2867,64 +2870,64 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>171</v>
+        <v>33</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>172</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>174</v>
+        <v>33</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>175</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>177</v>
@@ -2936,13 +2939,13 @@
         <v>179</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>181</v>
@@ -2951,13 +2954,13 @@
         <v>182</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>80</v>
+        <v>183</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>183</v>
+        <v>81</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="63" customHeight="1">
@@ -2965,85 +2968,85 @@
         <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AB16" s="4" t="s">
-        <v>185</v>
+        <v>33</v>
       </c>
       <c r="AC16" s="4" t="s">
         <v>186</v>
@@ -3055,7 +3058,7 @@
         <v>188</v>
       </c>
       <c r="AF16" s="4" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>